<commit_message>
Copy tidy focused on EventController and GameManager. ConfigStore now accessed via statics completely. Extensions added for getting config values. GetDescription and ToString for loading and saving beliefs now handled completely within Person class.
</commit_message>
<xml_diff>
--- a/stm-unity/Assets/Editor/Localization/SportsTeamManagerScenarioLocalization.xlsx
+++ b/stm-unity/Assets/Editor/Localization/SportsTeamManagerScenarioLocalization.xlsx
@@ -2975,10 +2975,10 @@
     <t>Neutral</t>
   </si>
   <si>
-    <t>StrongAgree</t>
-  </si>
-  <si>
-    <t>StrongDisagree</t>
+    <t>StronglyDisagree</t>
+  </si>
+  <si>
+    <t>StronglyAgree</t>
   </si>
 </sst>
 </file>
@@ -3329,6 +3329,54 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>971550</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="AutoShape 2"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="6353175" cy="6353175"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="r" b="b"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -3456,6 +3504,54 @@
           <a:ahLst/>
           <a:cxnLst/>
           <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>666750</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="AutoShape 2"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="6353175" cy="6353175"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="r" b="b"/>
           <a:pathLst/>
         </a:custGeom>
         <a:solidFill>
@@ -3617,6 +3713,54 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>238125</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>1171575</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="AutoShape 7"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="6353175" cy="6353175"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="r" b="b"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -3744,6 +3888,54 @@
           <a:ahLst/>
           <a:cxnLst/>
           <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>2438400</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="AutoShape 5"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="6353175" cy="6353175"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="r" b="b"/>
           <a:pathLst/>
         </a:custGeom>
         <a:solidFill>
@@ -4019,7 +4211,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -15446,7 +15638,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A17" sqref="A17"/>
+      <selection pane="bottomLeft" activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15" customHeight="1"/>
@@ -15536,7 +15728,7 @@
     </row>
     <row r="8" spans="1:3" ht="15.75" customHeight="1">
       <c r="A8" s="1" t="s">
-        <v>913</v>
+        <v>914</v>
       </c>
       <c r="B8" s="12" t="s">
         <v>419</v>
@@ -15569,7 +15761,7 @@
     </row>
     <row r="11" spans="1:3" ht="15.75" customHeight="1">
       <c r="A11" s="1" t="s">
-        <v>914</v>
+        <v>913</v>
       </c>
       <c r="B11" s="12" t="s">
         <v>425</v>

</xml_diff>